<commit_message>
moar data - wjec 2020
</commit_message>
<xml_diff>
--- a/sample-data/ingest-log.xlsx
+++ b/sample-data/ingest-log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>https://www.sqa.org.uk/sqa/files_ccc/ExamTimetable2020.pdf</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>OCR Exams - 2020.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.wjec.co.uk/exam-officers/Examination_Timetable_2020_Final_update_041219%20(2).pdf?language_id=1</t>
   </si>
 </sst>
 </file>
@@ -98,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -162,7 +165,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -511,7 +514,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -626,12 +629,19 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2">
+        <v>43863</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C6" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>